<commit_message>
data: tone frames for omission
</commit_message>
<xml_diff>
--- a/results/2023_08_09_omission_lfp_analysis/video_to_frame_and_subject.xlsx
+++ b/results/2023_08_09_omission_lfp_analysis/video_to_frame_and_subject.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26807"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26920"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_62D7479E5772F09A29C9EFE5FCBFF434EA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C90C448-2408-4D2C-B594-132E22551816}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="11_62D7479E5772F09A29C9EFE5FCBFF434EA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FB86871-2BD3-407C-8B99-F61167B4F840}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>file_path</t>
   </si>
@@ -48,6 +48,18 @@
     <t>all_subj</t>
   </si>
   <si>
+    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2.1.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>1.1_1.2</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2.1.fixed.2_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2.3.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
     <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1.1.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
@@ -60,25 +72,34 @@
     <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1.2.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1.2.fixed.2_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4.3.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>1.2_1.4</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4.3.fixed.2_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4.4.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
     <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1.1.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
-    <t>1.1_1.2</t>
-  </si>
-  <si>
     <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1.1.fixed.2_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
     <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1.2.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1.2.fixed.2_subj.round_1.id_corrected.h5</t>
+    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2.1.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2.1.fixed.2_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2.2.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
 </sst>
 </file>
@@ -442,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -470,69 +491,59 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="76.5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="76.5">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>32792</v>
-      </c>
-      <c r="C2" s="1">
-        <v>68495</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="76.5">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>41000</v>
       </c>
       <c r="C3" s="1">
-        <v>32316</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>79051</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.1000000000000001</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="76.5">
+    <row r="4" spans="1:5" ht="76.5">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
-        <v>32792</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>68495</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1.1000000000000001</v>
+        <v>39500</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="76.5">
+    <row r="5" spans="1:5" ht="76.5">
       <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>38957</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
@@ -540,119 +551,267 @@
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="76.5">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
-        <v>32860</v>
+        <v>32792</v>
       </c>
       <c r="C6" s="1">
-        <v>68288</v>
+        <v>68495</v>
       </c>
       <c r="D6" s="1">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="76.5">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
-        <v>2027</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>32240</v>
+        <v>32316</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="76.5">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
-        <v>32860</v>
+        <v>32792</v>
       </c>
       <c r="C8" s="1">
-        <v>68288</v>
+        <v>68495</v>
       </c>
       <c r="D8" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="76.5">
-      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" ht="76.5">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>32500</v>
+      </c>
+      <c r="C10" s="1">
+        <v>66320</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" ht="76.5">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>30000</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" ht="76.5">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
+        <v>32500</v>
+      </c>
+      <c r="C12" s="1">
+        <v>66006</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1">
       <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" ht="76.5">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <v>32860</v>
+      </c>
+      <c r="C14" s="1">
+        <v>68288</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" ht="76.5">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2027</v>
+      </c>
+      <c r="C15" s="1">
+        <v>32240</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" ht="76.5">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1">
+        <v>32860</v>
+      </c>
+      <c r="C16" s="1">
+        <v>68288</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1">
       <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" ht="76.5">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>35000</v>
+      </c>
+      <c r="C18">
+        <v>69768</v>
+      </c>
+      <c r="D18">
+        <v>1.4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="76.5">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>33500</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="76.5">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>34500</v>
+      </c>
+      <c r="C20">
+        <v>69684</v>
+      </c>
+      <c r="D20">
+        <v>1.2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:5">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:5">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:5">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:5">
       <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -660,28 +819,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="05f64c5e-7ec2-4cf0-a148-a77e53878df3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002C00C86E44419345A6E3C05C9040286D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75e447aa01971d87755e32be9f432ab5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="05f64c5e-7ec2-4cf0-a148-a77e53878df3" xmlns:ns3="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="128ff4447dd710e229a73405da0381bf" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002C00C86E44419345A6E3C05C9040286D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="47c6aa886674859c27167f35b4832502">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="05f64c5e-7ec2-4cf0-a148-a77e53878df3" xmlns:ns3="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d3bbbc1340a80856680a800397edf58e" ns2:_="" ns3:_="">
     <xsd:import namespace="05f64c5e-7ec2-4cf0-a148-a77e53878df3"/>
     <xsd:import namespace="66c7fa70-bb82-47de-8c9f-8b3ecea6303f"/>
     <xsd:element name="properties">
@@ -705,6 +844,7 @@
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -777,6 +917,11 @@
       </xsd:complexType>
     </xsd:element>
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="24" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -922,14 +1067,34 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="05f64c5e-7ec2-4cf0-a148-a77e53878df3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63C3B4A2-F48E-4DF2-B351-ACDCD6D0C529}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D770834-2B26-4F25-8CBB-FA13B41D6738}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE888698-F550-4D99-B643-806A083D1CEB}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31974A48-BEB3-433E-A58A-7476C55000D8}"/>
 </file>
</xml_diff>